<commit_message>
empty the search bar after go on result
</commit_message>
<xml_diff>
--- a/data/db_source/config.xlsx
+++ b/data/db_source/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannuaire/datannuaire_dev/public/data/db_source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D8776C-0D84-C043-8A95-0D227C3371B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332447E3-68EE-1745-A025-6938BDC6DFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3220" yWindow="500" windowWidth="25580" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,8 +156,54 @@
     <t>Les mots clés, ou tags, peuvent être attribués aux variables, aux datasets, aux institutions et aux dossiers.</t>
   </si>
   <si>
+    <t>about_doc</t>
+  </si>
+  <si>
+    <t>contact@datannur.com</t>
+  </si>
+  <si>
+    <t>La vue méta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
+Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de datannur.
+Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
+  </si>
+  <si>
+    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
+# datannur, le catalogue de données portable
+Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
+Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
+**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
+- **Facile** :
+Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
+- **Portable** :
+Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
+- **Complet** :
+Flexible, complet et structuré autour de 7 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
+- **Indépendant** :
+Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
+- **Sécurisé** :
+De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
+La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Fonctionnement
+datannur contient 7 concepts principaux. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
+mermaid( 
+  $dataset -.-&gt; intérieur
+  $dataset -.-&gt; extérieur
+);
+</t>
+  </si>
+  <si>
+    <t>Pour finir, certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.
+mermaid(
+  $doc &lt;--&gt; $institution
+  $doc &lt;--&gt; $folder
+  $doc &lt;--&gt; $dataset
+);</t>
+  </si>
+  <si>
     <t xml:space="preserve">#### Vision d'ensemble
-Voici les liens entre les 7 entités, à l'intérieur et l'extérieur des datasets.
+Voici les liens entre les 7 concepts, à l'intérieur et l'extérieur des datasets.
 mermaid(
   $folder $recursive
   $institution $recursive
@@ -180,53 +226,7 @@
 </t>
   </si>
   <si>
-    <t>Pour finir, certaines entités possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.
-mermaid(
-  $doc &lt;--&gt; $institution
-  $doc &lt;--&gt; $folder
-  $doc &lt;--&gt; $dataset
-);</t>
-  </si>
-  <si>
-    <t>about_doc</t>
-  </si>
-  <si>
-    <t>Certaines entités possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### Fonctionnement
-datannur contient 7 entités principales. On peut les diviser en deux catégories, partie intérieur et partie extérieur aux datasets. Le **dataset** représente une table de base de données ou un fichier de données (excel, csv, ...) sous forme de tableau (lignes et colonnes).
-mermaid( 
-  $dataset -.-&gt; intérieur
-  $dataset -.-&gt; extérieur
-);
-</t>
-  </si>
-  <si>
-    <t>contact@datannur.com</t>
-  </si>
-  <si>
-    <t>![main_banner not_rounded](data/img/main_banner{dark_mode}.png?v=1)
-# datannur, le catalogue de données portable
-Permet de **centraliser**, **rechercher** et **visualiser** les informations sur une collection de jeux de données
-Pour améliorer l’organisation des données et faciliter leur **partage** et leur **documentation**
-**Simple** et **flexible**, s’intègre rapidement dans tous types d’environnement
-- **Facile** :
-Aucune installation ou configuration nécessaire, aucun coût ou prérequis technique
-- **Portable** :
-Fonctionne partout (local, cloud, disque partagé), un simple dossier que l’on peut copier, déplacer, envoyer et ouvrir avec n’importe quel navigateur web
-- **Complet** :
-Flexible, complet et structuré autour de 6 concepts avec un niveau de détail important : Institution, Dossier, Mot clé, Dataset, Variable et Modalité
-- **Indépendant** :
-Le catalogue n’est qu’une interface pour visualiser les métadonnées, le processus de leur création et mise à jour est indépendant et sous votre contrôle
-- **Sécurisé** :
-De pars la séparation stricte entre les deux systèmes, l’application est isolée dans le navigateur, ne peut rien modifier sur la machine et ne pose ainsi aucun risque
-La version ici présente est un **prototype** en cours de développement et d'expérimentation. Les données utilisées sont fictives et uniquement à usage de test et de développement. Question ou suggestion : [contact@datannur.com](mailto:contact@datannur.com).</t>
-  </si>
-  <si>
-    <t>La vue méta représente les méta-méta-données, c’est-à-dire l'information sur les jeux de données internes au catalogue. 
-Cette vue apporte une synthèse générale sur le contenu du catalogue et permet de voir l'architecture de données de datannur.
-Pour vérifier l'intégriter de la base de données, cliquez sur ce [lien](?app_mode=check_db).</t>
+    <t>Certains concepts possèdent des docs (documents de type markdown ou pdf). Un **doc** peut être lié à une multitude de datasets, de dossiers et d'institutions, et inversement.</t>
   </si>
 </sst>
 </file>
@@ -653,10 +653,10 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="170" x14ac:dyDescent="0.2">
@@ -718,7 +718,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="404" x14ac:dyDescent="0.2">
@@ -726,7 +726,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="119" x14ac:dyDescent="0.2">
@@ -734,7 +734,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -803,10 +803,10 @@
     </row>
     <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>